<commit_message>
fix bug and format excel
</commit_message>
<xml_diff>
--- a/Backend/Format_file_DataImport.xlsx
+++ b/Backend/Format_file_DataImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Capstone_Project\Capstone-Warehouse\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64F36725-9247-40E4-9361-3C4CF616828B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC8C881-A0D6-464B-A20B-83B15B427F17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A21AED4A-F956-44B3-9F5D-A1D46A747D89}"/>
   </bookViews>
@@ -260,7 +260,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -315,9 +315,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="3" applyAlignment="1"/>
     <xf numFmtId="187" fontId="2" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
@@ -660,7 +659,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -674,12 +673,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -690,7 +689,7 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2"/>
@@ -704,7 +703,7 @@
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="23"/>
@@ -757,7 +756,7 @@
       <c r="G5" s="8"/>
       <c r="H5" s="9"/>
       <c r="I5" s="10">
-        <f>G5*E5-H5</f>
+        <f>G5*E5*(1-H5/100)</f>
         <v>0</v>
       </c>
     </row>
@@ -773,7 +772,7 @@
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
       <c r="I6" s="10">
-        <f t="shared" ref="I6:I8" si="0">G6*E6-H6</f>
+        <f t="shared" ref="I6:I8" si="0">G6*E6*(1-H6/100)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>